<commit_message>
Add lighting code and lighting videos
</commit_message>
<xml_diff>
--- a/Costs.xlsx
+++ b/Costs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\musil\projects\Embedded Plant Watering\embedded-plant-waterer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{074E961D-0BA8-4C41-AC56-5AD891B583A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB8B7840-4775-4FF2-B424-B5AEA0445180}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14265" yWindow="2460" windowWidth="14040" windowHeight="11205" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15720" yWindow="2280" windowWidth="12585" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Item</t>
   </si>
@@ -115,6 +115,12 @@
   </si>
   <si>
     <t>https://smile.amazon.com/gp/product/B07K6HXDH1/ref=ox_sc_act_title_2?smid=A2K4DGCC72N9AG&amp;psc=1</t>
+  </si>
+  <si>
+    <t>Plant and terra cota holder</t>
+  </si>
+  <si>
+    <t>Lowes</t>
   </si>
 </sst>
 </file>
@@ -453,7 +459,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -633,13 +639,27 @@
         <v>26</v>
       </c>
     </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>15</v>
+      </c>
+      <c r="D13" t="s">
+        <v>28</v>
+      </c>
+    </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C15">
-        <f>SUM(C2:C12)</f>
-        <v>154.5</v>
+        <f>SUM(C2:C13)</f>
+        <v>169.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>